<commit_message>
before big change to level
</commit_message>
<xml_diff>
--- a/Sheet drop.xlsx
+++ b/Sheet drop.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacob\AppData\Roaming\pico-8\carts\shallowend-pico8\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacob\AppData\Roaming\pico-8\carts\drop-p8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29F76C17-9C62-4B09-8627-A2AE84EEC50E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E95286A-96F6-404C-AF8A-2E0CFFABB6EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2F517386-D81F-4AF1-A133-9D983E9345C9}"/>
+    <workbookView xWindow="28680" yWindow="750" windowWidth="19440" windowHeight="15000" xr2:uid="{2F517386-D81F-4AF1-A133-9D983E9345C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Teleports" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="81">
   <si>
     <t>sx</t>
   </si>
@@ -56,54 +56,6 @@
     <t>Name</t>
   </si>
   <si>
-    <t>House enter</t>
-  </si>
-  <si>
-    <t>House exit1</t>
-  </si>
-  <si>
-    <t>House exit2</t>
-  </si>
-  <si>
-    <t>Slime enter</t>
-  </si>
-  <si>
-    <t>slime exit1</t>
-  </si>
-  <si>
-    <t>slime exit2</t>
-  </si>
-  <si>
-    <t>w twr e</t>
-  </si>
-  <si>
-    <t>w twr ex</t>
-  </si>
-  <si>
-    <t>w twr en</t>
-  </si>
-  <si>
-    <t>ghst ex</t>
-  </si>
-  <si>
-    <t>hog en</t>
-  </si>
-  <si>
-    <t>hog ex</t>
-  </si>
-  <si>
-    <t>ladder f21</t>
-  </si>
-  <si>
-    <t>ladder f23</t>
-  </si>
-  <si>
-    <t>ladder f32</t>
-  </si>
-  <si>
-    <t>ladder f12</t>
-  </si>
-  <si>
     <t>mus</t>
   </si>
   <si>
@@ -329,13 +281,7 @@
     <t>fail={"i thought you were more discerning than that. go away."},</t>
   </si>
   <si>
-    <t>secret entr</t>
-  </si>
-  <si>
-    <t>secret ex 1</t>
-  </si>
-  <si>
-    <t>secret ex 2</t>
+    <t>wave</t>
   </si>
 </sst>
 </file>
@@ -833,10 +779,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{968E7FE8-EAA6-4D7C-962A-12CADC7F5F87}">
-  <dimension ref="A1:X14"/>
+  <dimension ref="A1:R14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W9" sqref="W9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -854,495 +800,61 @@
     <col min="24" max="24" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K1" t="s">
-        <v>12</v>
-      </c>
-      <c r="L1" t="s">
-        <v>12</v>
-      </c>
-      <c r="M1" t="s">
-        <v>15</v>
-      </c>
-      <c r="N1" t="s">
-        <v>16</v>
-      </c>
-      <c r="O1" t="s">
-        <v>16</v>
-      </c>
-      <c r="P1" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>17</v>
-      </c>
-      <c r="R1" t="s">
-        <v>18</v>
-      </c>
-      <c r="S1" t="s">
-        <v>19</v>
-      </c>
-      <c r="T1" t="s">
-        <v>14</v>
-      </c>
-      <c r="U1" t="s">
-        <v>14</v>
-      </c>
-      <c r="V1" t="s">
-        <v>96</v>
-      </c>
-      <c r="W1" t="s">
-        <v>97</v>
-      </c>
-      <c r="X1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>11</v>
-      </c>
-      <c r="C2">
-        <v>123</v>
-      </c>
-      <c r="D2">
-        <v>124</v>
-      </c>
-      <c r="E2">
-        <v>51</v>
-      </c>
-      <c r="F2">
-        <v>107</v>
-      </c>
-      <c r="G2">
-        <v>108</v>
-      </c>
-      <c r="H2">
-        <v>91</v>
-      </c>
-      <c r="I2">
-        <v>92</v>
-      </c>
-      <c r="J2">
-        <v>93</v>
-      </c>
-      <c r="K2">
-        <v>115</v>
-      </c>
-      <c r="L2">
-        <v>116</v>
-      </c>
-      <c r="M2">
-        <v>99</v>
-      </c>
-      <c r="N2">
-        <v>115</v>
-      </c>
-      <c r="O2">
-        <v>116</v>
-      </c>
-      <c r="P2">
-        <v>125</v>
-      </c>
-      <c r="Q2">
-        <v>109</v>
-      </c>
-      <c r="R2">
-        <v>109</v>
-      </c>
-      <c r="S2">
-        <v>125</v>
-      </c>
-      <c r="T2">
-        <v>7</v>
-      </c>
-      <c r="U2">
-        <v>7</v>
-      </c>
-      <c r="V2">
-        <v>100</v>
-      </c>
-      <c r="W2">
-        <v>123</v>
-      </c>
-      <c r="X2">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3">
-        <v>11</v>
-      </c>
-      <c r="C3">
-        <v>7</v>
-      </c>
-      <c r="D3">
-        <v>7</v>
-      </c>
-      <c r="E3">
-        <v>5</v>
-      </c>
-      <c r="F3">
-        <v>23</v>
-      </c>
-      <c r="G3">
-        <v>23</v>
-      </c>
-      <c r="H3">
-        <v>10</v>
-      </c>
-      <c r="I3">
-        <v>10</v>
-      </c>
-      <c r="J3">
-        <v>10</v>
-      </c>
-      <c r="K3">
-        <v>15</v>
-      </c>
-      <c r="L3">
-        <v>15</v>
-      </c>
-      <c r="M3">
-        <v>29</v>
-      </c>
-      <c r="N3">
-        <v>23</v>
-      </c>
-      <c r="O3">
-        <v>23</v>
-      </c>
-      <c r="P3">
-        <v>21</v>
-      </c>
-      <c r="Q3">
-        <v>29</v>
-      </c>
-      <c r="R3">
-        <v>26</v>
-      </c>
-      <c r="S3">
-        <v>26</v>
-      </c>
-      <c r="T3">
-        <v>3</v>
-      </c>
-      <c r="U3">
-        <v>4</v>
-      </c>
-      <c r="V3">
-        <v>1</v>
-      </c>
-      <c r="W3">
-        <v>15</v>
-      </c>
-      <c r="X3">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4">
-        <v>984</v>
-      </c>
-      <c r="C4">
-        <v>88</v>
-      </c>
-      <c r="D4">
-        <v>88</v>
-      </c>
-      <c r="E4">
-        <f>108*8</f>
-        <v>864</v>
-      </c>
-      <c r="F4">
-        <v>408</v>
-      </c>
-      <c r="G4">
-        <v>408</v>
-      </c>
-      <c r="H4">
-        <v>928</v>
-      </c>
-      <c r="I4">
-        <v>928</v>
-      </c>
-      <c r="J4">
-        <v>928</v>
-      </c>
-      <c r="K4">
-        <f>92*8</f>
-        <v>736</v>
-      </c>
-      <c r="L4">
-        <f>92*8</f>
-        <v>736</v>
-      </c>
-      <c r="M4">
-        <v>928</v>
-      </c>
-      <c r="N4">
-        <v>792</v>
-      </c>
-      <c r="O4">
-        <v>792</v>
-      </c>
-      <c r="P4">
-        <v>872</v>
-      </c>
-      <c r="Q4">
-        <v>1000</v>
-      </c>
-      <c r="R4">
-        <v>1000</v>
-      </c>
-      <c r="S4">
-        <v>872</v>
-      </c>
-      <c r="T4">
-        <v>136</v>
-      </c>
-      <c r="U4">
-        <v>136</v>
-      </c>
-      <c r="V4">
-        <f>123*8</f>
-        <v>984</v>
-      </c>
-      <c r="W4">
-        <f>100*8</f>
-        <v>800</v>
-      </c>
-      <c r="X4">
-        <f>100*8</f>
-        <v>800</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5">
-        <v>48</v>
-      </c>
-      <c r="C5">
-        <v>100</v>
-      </c>
-      <c r="D5">
-        <v>100</v>
-      </c>
-      <c r="E5">
-        <f>22*8</f>
-        <v>176</v>
-      </c>
-      <c r="F5">
-        <v>48</v>
-      </c>
-      <c r="G5">
-        <v>48</v>
-      </c>
-      <c r="H5">
-        <v>112</v>
-      </c>
-      <c r="I5">
-        <v>112</v>
-      </c>
-      <c r="J5">
-        <v>112</v>
-      </c>
-      <c r="K5">
-        <f>12*8</f>
-        <v>96</v>
-      </c>
-      <c r="L5">
-        <f>12*8</f>
-        <v>96</v>
-      </c>
-      <c r="M5">
-        <v>176</v>
-      </c>
-      <c r="N5">
-        <v>240</v>
-      </c>
-      <c r="O5">
-        <v>240</v>
-      </c>
-      <c r="P5">
-        <f>28*8</f>
-        <v>224</v>
-      </c>
-      <c r="Q5">
-        <v>160</v>
-      </c>
-      <c r="R5">
-        <v>216</v>
-      </c>
-      <c r="S5">
-        <v>216</v>
-      </c>
-      <c r="T5">
-        <v>24</v>
-      </c>
-      <c r="U5">
-        <v>24</v>
-      </c>
-      <c r="V5">
-        <f>14*8</f>
-        <v>112</v>
-      </c>
-      <c r="W5">
-        <f>2*8</f>
-        <v>16</v>
-      </c>
-      <c r="X5">
-        <f>2*8</f>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6">
-        <v>-1</v>
-      </c>
-      <c r="C6">
-        <f>R11</f>
-        <v>32</v>
-      </c>
-      <c r="D6">
-        <f>R11</f>
-        <v>32</v>
-      </c>
-      <c r="E6">
-        <v>24</v>
-      </c>
-      <c r="F6">
-        <f>R11</f>
-        <v>32</v>
-      </c>
-      <c r="G6">
-        <f>R11</f>
-        <v>32</v>
-      </c>
-      <c r="H6">
-        <v>16</v>
-      </c>
-      <c r="I6">
-        <v>16</v>
-      </c>
-      <c r="J6">
-        <v>16</v>
-      </c>
-      <c r="K6">
-        <f>R11</f>
-        <v>32</v>
-      </c>
-      <c r="L6">
-        <f>R11</f>
-        <v>32</v>
-      </c>
-      <c r="M6">
-        <v>3</v>
-      </c>
-      <c r="N6">
-        <f>R11</f>
-        <v>32</v>
-      </c>
-      <c r="O6">
-        <f>R11</f>
-        <v>32</v>
-      </c>
-      <c r="P6">
-        <v>0</v>
-      </c>
-      <c r="Q6">
-        <v>0</v>
-      </c>
-      <c r="R6">
-        <v>0</v>
-      </c>
-      <c r="S6">
-        <v>0</v>
-      </c>
-      <c r="T6">
-        <f>R11</f>
-        <v>32</v>
-      </c>
-      <c r="U6">
-        <f>R11</f>
-        <v>32</v>
-      </c>
-      <c r="V6">
-        <v>-1</v>
-      </c>
-      <c r="W6">
-        <v>32</v>
-      </c>
-      <c r="X6">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C7" t="str">
         <f>_xlfn.CONCAT(A2&amp;"={",_xlfn.TEXTJOIN(",",TRUE,B2:AT2),"},")</f>
-        <v>sx={11,123,124,51,107,108,91,92,93,115,116,99,115,116,125,109,109,125,7,7,100,123,124},</v>
-      </c>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+        <v>sx={},</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C8" t="str">
         <f>_xlfn.CONCAT(A3&amp;"={",_xlfn.TEXTJOIN(",",TRUE,B3:AT3),"},")</f>
-        <v>sy={11,7,7,5,23,23,10,10,10,15,15,29,23,23,21,29,26,26,3,4,1,15,15},</v>
-      </c>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+        <v>sy={},</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C9" t="str">
         <f>_xlfn.CONCAT(A4&amp;"={",_xlfn.TEXTJOIN(",",TRUE,B4:AT4),"},")</f>
-        <v>nx={984,88,88,864,408,408,928,928,928,736,736,928,792,792,872,1000,1000,872,136,136,984,800,800},</v>
-      </c>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+        <v>nx={},</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C10" t="str">
         <f>_xlfn.CONCAT(A5&amp;"={",_xlfn.TEXTJOIN(",",TRUE,B5:AT5),"},")</f>
-        <v>ny={48,100,100,176,48,48,112,112,112,96,96,176,240,240,224,160,216,216,24,24,112,16,16},</v>
+        <v>ny={},</v>
       </c>
       <c r="M10">
         <v>872</v>
@@ -1352,13 +864,13 @@
         <v>109</v>
       </c>
       <c r="R10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C11" t="str">
         <f>_xlfn.CONCAT(A6&amp;"={",_xlfn.TEXTJOIN(",",TRUE,B6:AT6),"},")</f>
-        <v>mus={-1,32,32,24,32,32,16,16,16,32,32,3,32,32,0,0,0,0,32,32,-1,32,32},</v>
+        <v>mus={},</v>
       </c>
       <c r="M11">
         <f>28*8</f>
@@ -1371,7 +883,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="M12">
         <v>1000</v>
       </c>
@@ -1379,7 +891,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="M13">
         <v>216</v>
       </c>
@@ -1387,7 +899,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="M14">
         <v>872</v>
       </c>
@@ -1422,57 +934,57 @@
         <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="D1" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="E1" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="F1" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="G1" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="H1" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="I1" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="J1" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="K1" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="L1" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="M1" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="N1" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="O1" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="P1" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="Q1" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="B2">
         <v>6</v>
@@ -1525,7 +1037,7 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="B3">
         <v>25</v>
@@ -1578,7 +1090,7 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="B4">
         <v>30</v>
@@ -1665,7 +1177,7 @@
         <v>={}</v>
       </c>
       <c r="H10" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="I10">
         <f>I9*8</f>
@@ -1949,7 +1461,7 @@
   <sheetData>
     <row r="1" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B1" s="12" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="C1" s="13"/>
       <c r="D1" s="13"/>
@@ -1959,107 +1471,107 @@
     </row>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" s="15" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="15" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="G3" s="17" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="17" t="s">
         <v>33</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="E4" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="F4" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="G4" s="17" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="16" t="s">
-        <v>50</v>
-      </c>
       <c r="D5" s="16" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="G5" s="17" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="15" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="G6" s="17" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="15" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="C7" s="16">
         <v>1</v>
@@ -2087,10 +1599,10 @@
     </row>
     <row r="9" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B9" s="15" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="D9" s="16"/>
       <c r="E9" s="16"/>
@@ -2099,10 +1611,10 @@
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" s="15" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="D10" s="16"/>
       <c r="E10" s="16"/>
@@ -2123,7 +1635,7 @@
         <v>question={"what is the best way to enter a room?","what is a ghost's favorite food?","riddle time: what month of the year has 28 days?","alright, what is 6/2(1+2)?","i weigh 90 pounds plus half my weight. how much do i weigh?"},</v>
       </c>
       <c r="D12" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="G12" s="6"/>
     </row>
@@ -2133,7 +1645,7 @@
         <v>answer_a={"knock","spook-hetti","january. sometimes.","nine!","90 pounds"},</v>
       </c>
       <c r="D13" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="G13" s="6"/>
     </row>
@@ -2143,7 +1655,7 @@
         <v>answer_b={"kick the door open.","nothing. they're dead.","all of them","one","180 pounds"},</v>
       </c>
       <c r="D14" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="G14" s="6"/>
     </row>
@@ -2153,7 +1665,7 @@
         <v>reply_a={"that one was too easy","ahh, a man of culture. let's continue.","uh, you are sort of correct. but not really. not even close.","math is boring anyway…","funny, no."},</v>
       </c>
       <c r="D15" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="G15" s="6"/>
     </row>
@@ -2163,7 +1675,7 @@
         <v>reply_b={"see. i knew it. jerk.","wow, way to be that guy.","aha! yes. stealth answer.","got you! math is amazing.","(if i weighed anything you would be correct)"},</v>
       </c>
       <c r="D16" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="G16" s="6"/>
     </row>
@@ -2174,7 +1686,7 @@
       </c>
       <c r="C17" s="8"/>
       <c r="D17" s="8" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
@@ -2182,7 +1694,7 @@
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="10" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="C20" s="13"/>
       <c r="D20" s="13"/>
@@ -2192,107 +1704,107 @@
     </row>
     <row r="21" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B21" s="11" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="D21" s="16" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="E21" s="16" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="F21" s="16" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="G21" s="17" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="11" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="E22" s="16" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="F22" s="16" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="G22" s="17" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="11" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="D23" s="16" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="E23" s="16" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="F23" s="16" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="G23" s="17" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
     </row>
     <row r="24" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B24" s="11" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="E24" s="16" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="F24" s="16" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="G24" s="17" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
     </row>
     <row r="25" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B25" s="11" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="D25" s="16" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="E25" s="16" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="F25" s="16" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="G25" s="17" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="11" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="C26" s="16">
         <v>2</v>
@@ -2320,10 +1832,10 @@
     </row>
     <row r="28" spans="2:7" ht="90" x14ac:dyDescent="0.25">
       <c r="B28" s="11" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="D28" s="16"/>
       <c r="E28" s="16"/>
@@ -2332,10 +1844,10 @@
     </row>
     <row r="29" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B29" s="11" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="D29" s="16"/>
       <c r="E29" s="16"/>
@@ -2352,7 +1864,7 @@
         <v>question={"why do you disturb me?","your brother tried to black mail me before dying... defame me to the town.","i asked him why he was doing this. he started waving his sword around.","he started destroying my research and then he... well, you know.","why have you come to my domain?"},</v>
       </c>
       <c r="D31" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="G31" s="6"/>
     </row>
@@ -2362,7 +1874,7 @@
         <v>answer_a={"you will pay swine!","he would never.","please continue.","why care about the books?","i need your pendant."},</v>
       </c>
       <c r="D32" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="G32" s="6"/>
     </row>
@@ -2372,7 +1884,7 @@
         <v>answer_b={"what does your research entail?","i've been getting that vibe...","you deserved it.","i think you murdered him.","i needed to find the murderer."},</v>
       </c>
       <c r="D33" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="G33" s="6"/>
     </row>
@@ -2382,7 +1894,7 @@
         <v>reply_a={"someone else died trying to kill me. tripped on my spiky throw rug and...","why would i lie about it? he is dead regardless.","you seem different then him.","they contain all my written notes on the subject of the gate.","it's yours, i finished my research on it earlier."},</v>
       </c>
       <c r="D34" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="G34" s="6"/>
     </row>
@@ -2392,7 +1904,7 @@
         <v>reply_b={"i'm testing this pendant to see if it reacts with a part of the door.","he said he would leave me alone if i paid tribute to him.","maybe so, but i can't help how i was born, same as you.","maybe i did. i do feel guilty about my home setup. it is not safe for tiny humans.","well, you are welcome to destroy my doormat."},</v>
       </c>
       <c r="D35" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="G35" s="6"/>
     </row>
@@ -2402,7 +1914,7 @@
         <v>Correct={2,2,1,1,1},</v>
       </c>
       <c r="D36" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="G36" s="6"/>
     </row>

</xml_diff>